<commit_message>
feat: Add multi-platform support and cross-platform compatibility
- Add platform detection system with utils/platform_utils.py
- Implement cross-platform ChromeDriver management
- Update browser configuration for different OS (Windows/Linux/macOS)
- Add requirements.txt and setup.py for easy installation
- Create INSTALL.md with platform-specific setup instructions
- Fix circular import issues between modules
- Remove hardcoded ChromeDriver paths
- Add automatic Chrome browser detection
- Improve file path handling for cross-platform compatibility
- Update configuration to use platform-specific settings
</commit_message>
<xml_diff>
--- a/data/character_info.xlsx
+++ b/data/character_info.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>玩家</t>
   </si>
@@ -43,54 +43,6 @@
     <t>职业</t>
   </si>
   <si>
-    <t>亮仔</t>
-  </si>
-  <si>
-    <t>嘭地一声</t>
-  </si>
-  <si>
-    <t>回音山</t>
-  </si>
-  <si>
-    <t>德鲁伊</t>
-  </si>
-  <si>
-    <t>邪能肖战</t>
-  </si>
-  <si>
-    <t>恶魔猎手</t>
-  </si>
-  <si>
-    <t>吴工</t>
-  </si>
-  <si>
-    <t>体育老师</t>
-  </si>
-  <si>
-    <t>通灵学院</t>
-  </si>
-  <si>
-    <t>战士</t>
-  </si>
-  <si>
-    <t>邀月</t>
-  </si>
-  <si>
-    <t>丽丽（四川）</t>
-  </si>
-  <si>
-    <t>骑士</t>
-  </si>
-  <si>
-    <t>黑魔仙豹哥</t>
-  </si>
-  <si>
-    <t>死亡之翼</t>
-  </si>
-  <si>
-    <t>死亡骑士</t>
-  </si>
-  <si>
     <t>段总</t>
   </si>
   <si>
@@ -101,87 +53,6 @@
   </si>
   <si>
     <t>盗贼</t>
-  </si>
-  <si>
-    <t>飞翔的潼瑜</t>
-  </si>
-  <si>
-    <t>舒总</t>
-  </si>
-  <si>
-    <t>Fountine</t>
-  </si>
-  <si>
-    <t>图拉扬</t>
-  </si>
-  <si>
-    <t>法师</t>
-  </si>
-  <si>
-    <t>天灵浴血</t>
-  </si>
-  <si>
-    <t>诺兹多姆</t>
-  </si>
-  <si>
-    <t>统皇</t>
-  </si>
-  <si>
-    <t>焦糖扁可颂</t>
-  </si>
-  <si>
-    <t>斯坦索姆</t>
-  </si>
-  <si>
-    <t>本间芽衣芓</t>
-  </si>
-  <si>
-    <t>巨奶</t>
-  </si>
-  <si>
-    <t>傻瓜观测</t>
-  </si>
-  <si>
-    <t>影之哀伤</t>
-  </si>
-  <si>
-    <t>牧师</t>
-  </si>
-  <si>
-    <t>捷教授</t>
-  </si>
-  <si>
-    <t>四个自信</t>
-  </si>
-  <si>
-    <t>蔡圣</t>
-  </si>
-  <si>
-    <t>莱恩弗尔特</t>
-  </si>
-  <si>
-    <t>神圣之歌</t>
-  </si>
-  <si>
-    <t>猎人</t>
-  </si>
-  <si>
-    <t>亚妮艾丝</t>
-  </si>
-  <si>
-    <t>亚里欧斯</t>
-  </si>
-  <si>
-    <t>元神</t>
-  </si>
-  <si>
-    <t>阿瘫</t>
-  </si>
-  <si>
-    <t>霜之哀伤</t>
-  </si>
-  <si>
-    <t>萨满</t>
   </si>
 </sst>
 </file>
@@ -1112,13 +983,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
     <col min="2" max="2" width="14.3333333333333" customWidth="1"/>
   </cols>
@@ -1149,230 +1020,6 @@
       </c>
       <c r="D2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add new features and update data
</commit_message>
<xml_diff>
--- a/data/character_info.xlsx
+++ b/data/character_info.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>玩家</t>
   </si>
@@ -43,6 +43,54 @@
     <t>职业</t>
   </si>
   <si>
+    <t>亮仔</t>
+  </si>
+  <si>
+    <t>嘭地一声</t>
+  </si>
+  <si>
+    <t>回音山</t>
+  </si>
+  <si>
+    <t>德鲁伊</t>
+  </si>
+  <si>
+    <t>邪能肖战</t>
+  </si>
+  <si>
+    <t>恶魔猎手</t>
+  </si>
+  <si>
+    <t>吴工</t>
+  </si>
+  <si>
+    <t>体育老师</t>
+  </si>
+  <si>
+    <t>通灵学院</t>
+  </si>
+  <si>
+    <t>战士</t>
+  </si>
+  <si>
+    <t>邀月</t>
+  </si>
+  <si>
+    <t>丽丽（四川）</t>
+  </si>
+  <si>
+    <t>骑士</t>
+  </si>
+  <si>
+    <t>黑魔仙豹哥</t>
+  </si>
+  <si>
+    <t>死亡之翼</t>
+  </si>
+  <si>
+    <t>死亡骑士</t>
+  </si>
+  <si>
     <t>段总</t>
   </si>
   <si>
@@ -53,6 +101,87 @@
   </si>
   <si>
     <t>盗贼</t>
+  </si>
+  <si>
+    <t>飞翔的潼瑜</t>
+  </si>
+  <si>
+    <t>舒总</t>
+  </si>
+  <si>
+    <t>Fountine</t>
+  </si>
+  <si>
+    <t>图拉扬</t>
+  </si>
+  <si>
+    <t>法师</t>
+  </si>
+  <si>
+    <t>天灵浴血</t>
+  </si>
+  <si>
+    <t>诺兹多姆</t>
+  </si>
+  <si>
+    <t>统皇</t>
+  </si>
+  <si>
+    <t>焦糖扁可颂</t>
+  </si>
+  <si>
+    <t>斯坦索姆</t>
+  </si>
+  <si>
+    <t>本间芽衣芓</t>
+  </si>
+  <si>
+    <t>巨奶</t>
+  </si>
+  <si>
+    <t>傻瓜观测</t>
+  </si>
+  <si>
+    <t>影之哀伤</t>
+  </si>
+  <si>
+    <t>牧师</t>
+  </si>
+  <si>
+    <t>捷教授</t>
+  </si>
+  <si>
+    <t>四个自信</t>
+  </si>
+  <si>
+    <t>蔡圣</t>
+  </si>
+  <si>
+    <t>莱恩弗尔特</t>
+  </si>
+  <si>
+    <t>神圣之歌</t>
+  </si>
+  <si>
+    <t>猎人</t>
+  </si>
+  <si>
+    <t>亚妮艾丝</t>
+  </si>
+  <si>
+    <t>亚里欧斯</t>
+  </si>
+  <si>
+    <t>元神</t>
+  </si>
+  <si>
+    <t>阿瘫</t>
+  </si>
+  <si>
+    <t>霜之哀伤</t>
+  </si>
+  <si>
+    <t>萨满</t>
   </si>
 </sst>
 </file>
@@ -983,13 +1112,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
     <col min="2" max="2" width="14.3333333333333" customWidth="1"/>
   </cols>
@@ -1020,6 +1149,230 @@
       </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add player and class filters to character stats
</commit_message>
<xml_diff>
--- a/data/character_info.xlsx
+++ b/data/character_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>骑士</t>
+          <t>圣骑士</t>
         </is>
       </c>
     </row>
@@ -590,171 +590,171 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>巨奶</t>
+          <t>屯狗</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>傻瓜观测</t>
+          <t>屯屯宝宝</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>影之哀伤</t>
+          <t>斯坦索姆</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>牧师</t>
+          <t>猎人</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>捷教授</t>
+          <t>巨奶</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>四个自信</t>
+          <t>傻瓜观测</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>回音山</t>
+          <t>影之哀伤</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>法师</t>
+          <t>牧师</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>段总</t>
+          <t>巨奶</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>生锈的斩牛刀</t>
+          <t>天赐祝福</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>伊森利恩</t>
+          <t>米奈希尔</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>盗贼</t>
+          <t>圣骑士</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>段总</t>
+          <t>捷教授</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>飞翔的潼瑜</t>
+          <t>四个自信</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>伊森利恩</t>
+          <t>回音山</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>死亡骑士</t>
+          <t>法师</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>统皇</t>
+          <t>昶狂</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>焦糖扁可颂</t>
+          <t>冲锋先看路</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>斯坦索姆</t>
+          <t>霜之哀伤</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>骑士</t>
+          <t>战士</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>统皇</t>
+          <t>昶狂</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>本间芽衣芓</t>
+          <t>战复慢点起</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>斯坦索姆</t>
+          <t>霜之哀伤</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>战士</t>
+          <t>死亡骑士</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>舒总</t>
+          <t>段总</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Fountine</t>
+          <t>生锈的斩牛刀</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>图拉扬</t>
+          <t>伊森利恩</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>法师</t>
+          <t>盗贼</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>舒总</t>
+          <t>段总</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>天灵浴血</t>
+          <t>飞翔的潼瑜</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>诺兹多姆</t>
+          <t>伊森利恩</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -766,66 +766,264 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>蔡圣</t>
+          <t>统皇</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>莱恩弗尔特</t>
+          <t>焦糖扁可颂</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>神圣之歌</t>
+          <t>斯坦索姆</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>猎人</t>
+          <t>圣骑士</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>蔡圣</t>
+          <t>统皇</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>亚妮艾丝</t>
+          <t>本间芽衣芓</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>神圣之歌</t>
+          <t>斯坦索姆</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>牧师</t>
+          <t>战士</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>统皇</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>生命众筹</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>斯坦索姆</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>死亡骑士</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>统皇</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>亻沈默</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>图拉扬</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>法师</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>舒总</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Fountine</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>图拉扬</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>法师</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>舒总</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>天灵浴血</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>诺兹多姆</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>死亡骑士</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>舒总</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>霜满天丶</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>图拉扬</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>恶魔猎手</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>蔡圣</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>莱恩弗尔特</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>神圣之歌</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>猎人</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
         <is>
           <t>蔡圣</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>亚妮艾丝</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
         <is>
           <t>神圣之歌</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>牧师</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>蔡圣</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>亚里欧斯</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>神圣之歌</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
         <is>
           <t>恶魔猎手</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>蔡圣</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>伊格瑞特</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>神圣之歌</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>德鲁伊</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>蔡圣</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>萨里西翁</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>神圣之歌</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>萨满</t>
         </is>
       </c>
     </row>

</xml_diff>